<commit_message>
Simplified the trajectory plot
</commit_message>
<xml_diff>
--- a/Artillery/Shiny_Shots/shots/M795.xlsx
+++ b/Artillery/Shiny_Shots/shots/M795.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RStudio\MyProjects\Artillery\Shiny_Shots\shots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2008D40D-C835-47C7-8148-F90E4AE85AB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7030D72B-A0B6-4A6C-9084-9A67431D27AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{ACD2B132-6E61-4758-88E4-4B02781318D4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="25">
   <si>
     <t>DFS</t>
   </si>
@@ -2499,11 +2499,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84C41F4F-EBAC-4919-9985-D9EB2643DC57}">
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2841,7 +2841,7 @@
         <v>204</v>
       </c>
       <c r="L7">
-        <f t="shared" ref="L7:L14" si="6">K7-C7</f>
+        <f t="shared" ref="L7:L15" si="6">K7-C7</f>
         <v>102.3</v>
       </c>
       <c r="M7">
@@ -2927,27 +2927,33 @@
       </c>
       <c r="G9">
         <f t="shared" si="3"/>
-        <v>-4.1666556537087587</v>
+        <v>2.3879867339872851E-2</v>
       </c>
       <c r="H9">
         <f t="shared" si="4"/>
-        <v>-2.1666556537087591</v>
+        <v>-2.0603451764385446E-2</v>
       </c>
       <c r="J9">
         <f t="shared" si="5"/>
         <v>61.042317554675947</v>
       </c>
+      <c r="K9">
+        <v>255.8</v>
+      </c>
       <c r="L9">
         <f t="shared" si="6"/>
-        <v>-193.3</v>
+        <v>62.5</v>
       </c>
       <c r="M9">
         <f t="shared" si="7"/>
         <v>-61.042317554675947</v>
       </c>
+      <c r="N9">
+        <v>131</v>
+      </c>
       <c r="O9">
         <f t="shared" si="8"/>
-        <v>-193.3</v>
+        <v>-62.300000000000011</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -2957,29 +2963,47 @@
       <c r="B10">
         <v>6000</v>
       </c>
+      <c r="C10">
+        <v>246.2</v>
+      </c>
+      <c r="D10">
+        <v>18</v>
+      </c>
+      <c r="E10">
+        <v>7</v>
+      </c>
+      <c r="F10">
+        <v>426</v>
+      </c>
       <c r="G10">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>4.5449460719777471E-2</v>
       </c>
       <c r="H10">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>-3.3658677328201145E-2</v>
       </c>
       <c r="J10">
         <f t="shared" si="5"/>
         <v>50.887204019764404</v>
       </c>
+      <c r="K10">
+        <v>299.39999999999998</v>
+      </c>
       <c r="L10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>53.199999999999989</v>
       </c>
       <c r="M10">
         <f t="shared" si="7"/>
         <v>-50.887204019764404</v>
       </c>
+      <c r="N10">
+        <v>193.6</v>
+      </c>
       <c r="O10">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>-52.599999999999994</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -2989,29 +3013,47 @@
       <c r="B11">
         <v>7000</v>
       </c>
+      <c r="C11">
+        <v>304.7</v>
+      </c>
+      <c r="D11">
+        <v>22</v>
+      </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>626</v>
+      </c>
       <c r="G11">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>6.8140247417609615E-2</v>
       </c>
       <c r="H11">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>-5.8971661602865412E-2</v>
       </c>
       <c r="J11">
         <f t="shared" si="5"/>
         <v>43.627229769370231</v>
       </c>
+      <c r="K11">
+        <v>351.3</v>
+      </c>
       <c r="L11">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>46.600000000000023</v>
       </c>
       <c r="M11">
         <f t="shared" si="7"/>
         <v>-43.627229769370231</v>
       </c>
+      <c r="N11">
+        <v>258.5</v>
+      </c>
       <c r="O11">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>-46.199999999999989</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -3021,29 +3063,47 @@
       <c r="B12">
         <v>8000</v>
       </c>
+      <c r="C12">
+        <v>370.1</v>
+      </c>
+      <c r="D12">
+        <v>26</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>884</v>
+      </c>
       <c r="G12">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>0.11054953557288512</v>
       </c>
       <c r="H12">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>-0.10007265316182075</v>
       </c>
       <c r="J12">
         <f t="shared" si="5"/>
         <v>38.179296503084508</v>
       </c>
+      <c r="K12">
+        <v>412.5</v>
+      </c>
       <c r="L12">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>42.399999999999977</v>
       </c>
       <c r="M12">
         <f t="shared" si="7"/>
         <v>-38.179296503084508</v>
       </c>
+      <c r="N12">
+        <v>328.1</v>
+      </c>
       <c r="O12">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>-42</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -3053,29 +3113,47 @@
       <c r="B13">
         <v>9000</v>
       </c>
+      <c r="C13">
+        <v>446.3</v>
+      </c>
+      <c r="D13">
+        <v>31</v>
+      </c>
+      <c r="E13">
+        <v>13</v>
+      </c>
+      <c r="F13">
+        <v>1226</v>
+      </c>
       <c r="G13">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>0.19031878268271962</v>
       </c>
       <c r="H13">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>-0.19031878268272129</v>
       </c>
       <c r="J13">
         <f t="shared" si="5"/>
         <v>33.940487697713351</v>
       </c>
+      <c r="K13">
+        <v>486.7</v>
+      </c>
       <c r="L13">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>40.399999999999977</v>
       </c>
       <c r="M13">
         <f t="shared" si="7"/>
         <v>-33.940487697713351</v>
       </c>
+      <c r="N13">
+        <v>405.9</v>
+      </c>
       <c r="O13">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>-40.400000000000034</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -3085,29 +3163,47 @@
       <c r="B14">
         <v>10000</v>
       </c>
+      <c r="C14">
+        <v>540.70000000000005</v>
+      </c>
+      <c r="D14">
+        <v>36</v>
+      </c>
+      <c r="E14">
+        <v>16</v>
+      </c>
+      <c r="F14">
+        <v>1708</v>
+      </c>
       <c r="G14">
         <f t="shared" si="3"/>
-        <v>-1</v>
+        <v>0.44032849826147868</v>
       </c>
       <c r="H14">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>-0.37158554720809106</v>
       </c>
       <c r="J14">
         <f t="shared" si="5"/>
         <v>30.548586696097015</v>
       </c>
+      <c r="K14">
+        <v>584.70000000000005</v>
+      </c>
       <c r="L14">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="M14">
         <f t="shared" si="7"/>
         <v>-30.548586696097015</v>
       </c>
+      <c r="N14">
+        <v>498.8</v>
+      </c>
       <c r="O14">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>-41.900000000000034</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -3115,7 +3211,49 @@
         <v>16</v>
       </c>
       <c r="B15">
-        <v>3000</v>
+        <v>4000</v>
+      </c>
+      <c r="C15">
+        <v>79.099999999999994</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>87</v>
+      </c>
+      <c r="G15">
+        <f t="shared" ref="G15" si="9">(L15-J15)/ABS(J15)</f>
+        <v>3.2574426955328671E-3</v>
+      </c>
+      <c r="H15">
+        <f t="shared" ref="H15" si="10">(O15-M15)/ABS(M15)</f>
+        <v>-1.945995058022255E-3</v>
+      </c>
+      <c r="J15">
+        <f t="shared" ref="J15" si="11">ATAN(300/B15)*3200/PI()</f>
+        <v>76.25161473456032</v>
+      </c>
+      <c r="K15">
+        <v>155.6</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="6"/>
+        <v>76.5</v>
+      </c>
+      <c r="M15">
+        <f t="shared" ref="M15" si="12">ATAN(-300/B15)*3200/PI()</f>
+        <v>-76.25161473456032</v>
+      </c>
+      <c r="N15">
+        <v>2.7</v>
+      </c>
+      <c r="O15">
+        <f t="shared" ref="O15" si="13">N15-C15</f>
+        <v>-76.399999999999991</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -3125,25 +3263,151 @@
       <c r="B16">
         <v>5000</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>106</v>
+      </c>
+      <c r="D16">
+        <v>11</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <v>151</v>
+      </c>
+      <c r="G16">
+        <f t="shared" ref="G16:G23" si="14">(L16-J16)/ABS(J16)</f>
+        <v>5.8595816746911823E-3</v>
+      </c>
+      <c r="H16">
+        <f t="shared" ref="H16:H23" si="15">(O16-M16)/ABS(M16)</f>
+        <v>-9.4495831145972246E-4</v>
+      </c>
+      <c r="J16">
+        <f t="shared" ref="J16:J23" si="16">ATAN(300/B16)*3200/PI()</f>
+        <v>61.042317554675947</v>
+      </c>
+      <c r="K16">
+        <v>167.4</v>
+      </c>
+      <c r="L16">
+        <f t="shared" ref="L16:L23" si="17">K16-C16</f>
+        <v>61.400000000000006</v>
+      </c>
+      <c r="M16">
+        <f t="shared" ref="M16:M23" si="18">ATAN(-300/B16)*3200/PI()</f>
+        <v>-61.042317554675947</v>
+      </c>
+      <c r="N16">
+        <v>44.9</v>
+      </c>
+      <c r="O16">
+        <f t="shared" ref="O16:O23" si="19">N16-C16</f>
+        <v>-61.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17">
         <f>ROUND(AVERAGE(B19,B15),-3)</f>
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>7000</v>
+      </c>
+      <c r="C17">
+        <v>172.2</v>
+      </c>
+      <c r="D17">
+        <v>17</v>
+      </c>
+      <c r="E17">
+        <v>6</v>
+      </c>
+      <c r="F17">
+        <v>366</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="14"/>
+        <v>1.0836586075463207E-2</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="15"/>
+        <v>-8.5444396217768306E-3</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="16"/>
+        <v>43.627229769370231</v>
+      </c>
+      <c r="K17">
+        <v>216.3</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="17"/>
+        <v>44.100000000000023</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="18"/>
+        <v>-43.627229769370231</v>
+      </c>
+      <c r="N17">
+        <v>128.19999999999999</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="19"/>
+        <v>-44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18">
         <v>8000</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>211.9</v>
+      </c>
+      <c r="D18">
+        <v>20</v>
+      </c>
+      <c r="E18">
+        <v>7</v>
+      </c>
+      <c r="F18">
+        <v>529</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="14"/>
+        <v>1.8876814476067462E-2</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="15"/>
+        <v>-1.6257593873301373E-2</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="16"/>
+        <v>38.179296503084508</v>
+      </c>
+      <c r="K18">
+        <v>250.8</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="17"/>
+        <v>38.900000000000006</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="18"/>
+        <v>-38.179296503084508</v>
+      </c>
+      <c r="N18">
+        <v>173.1</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="19"/>
+        <v>-38.800000000000011</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -3151,16 +3415,100 @@
         <f>ROUND(AVERAGE(B23,B15),-3)</f>
         <v>9000</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>256.10000000000002</v>
+      </c>
+      <c r="D19">
+        <v>24</v>
+      </c>
+      <c r="E19">
+        <v>9</v>
+      </c>
+      <c r="F19">
+        <v>736</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="14"/>
+        <v>3.4163100796124793E-2</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="15"/>
+        <v>-2.5324099934620783E-2</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="16"/>
+        <v>33.940487697713351</v>
+      </c>
+      <c r="K19">
+        <v>291.2</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="17"/>
+        <v>35.099999999999966</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="18"/>
+        <v>-33.940487697713351</v>
+      </c>
+      <c r="N19">
+        <v>221.3</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="19"/>
+        <v>-34.800000000000011</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
       <c r="B20">
         <v>10000</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>305.10000000000002</v>
+      </c>
+      <c r="D20">
+        <v>27</v>
+      </c>
+      <c r="E20">
+        <v>10</v>
+      </c>
+      <c r="F20">
+        <v>994</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="14"/>
+        <v>5.4058582818627202E-2</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="15"/>
+        <v>-4.4238161239573158E-2</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="16"/>
+        <v>30.548586696097015</v>
+      </c>
+      <c r="K20">
+        <v>337.3</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="17"/>
+        <v>32.199999999999989</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="18"/>
+        <v>-30.548586696097015</v>
+      </c>
+      <c r="N20">
+        <v>273.2</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="19"/>
+        <v>-31.900000000000034</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -3168,96 +3516,490 @@
         <f>ROUND(AVERAGE(B23,B19),-3)</f>
         <v>12000</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>420.6</v>
+      </c>
+      <c r="D21">
+        <v>36</v>
+      </c>
+      <c r="E21">
+        <v>15</v>
+      </c>
+      <c r="F21">
+        <v>1702</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="14"/>
+        <v>0.13120893548428586</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="15"/>
+        <v>-0.11549770026922944</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="16"/>
+        <v>25.459487718482603</v>
+      </c>
+      <c r="K21">
+        <v>449.4</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="17"/>
+        <v>28.799999999999955</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="18"/>
+        <v>-25.459487718482603</v>
+      </c>
+      <c r="N21">
+        <v>392.2</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="19"/>
+        <v>-28.400000000000034</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
       <c r="B22">
         <v>13000</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>490</v>
+      </c>
+      <c r="D22">
+        <v>41</v>
+      </c>
+      <c r="E22">
+        <v>17</v>
+      </c>
+      <c r="F22">
+        <v>2191</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="14"/>
+        <v>0.26798855024841994</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="15"/>
+        <v>-0.15735867673681411</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="16"/>
+        <v>23.501789502879692</v>
+      </c>
+      <c r="K22">
+        <v>519.79999999999995</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="17"/>
+        <v>29.799999999999955</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="18"/>
+        <v>-23.501789502879692</v>
+      </c>
+      <c r="N22">
+        <v>462.8</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="19"/>
+        <v>-27.199999999999989</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>16</v>
       </c>
       <c r="B23">
         <v>14000</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>577.9</v>
+      </c>
+      <c r="D23">
+        <v>47</v>
+      </c>
+      <c r="E23">
+        <v>21</v>
+      </c>
+      <c r="F23">
+        <v>2847</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="14"/>
+        <v>0.47088313412861332</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="15"/>
+        <v>-0.38840370604663194</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="16"/>
+        <v>21.823623682391897</v>
+      </c>
+      <c r="K23">
+        <v>610</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="17"/>
+        <v>32.100000000000023</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="18"/>
+        <v>-21.823623682391897</v>
+      </c>
+      <c r="N23">
+        <v>547.6</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="19"/>
+        <v>-30.299999999999955</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>17</v>
       </c>
       <c r="B24">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4000</v>
+      </c>
+      <c r="C24">
+        <v>53</v>
+      </c>
+      <c r="D24">
+        <v>6</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>58</v>
+      </c>
+      <c r="G24">
+        <f t="shared" ref="G24:G31" si="20">(L24-J24)/ABS(J24)</f>
+        <v>6.3454742051201546E-4</v>
+      </c>
+      <c r="H24">
+        <f t="shared" ref="H24:H31" si="21">(O24-M24)/ABS(M24)</f>
+        <v>-1.9459950580224413E-3</v>
+      </c>
+      <c r="J24">
+        <f t="shared" ref="J24:J31" si="22">ATAN(300/B24)*3200/PI()</f>
+        <v>76.25161473456032</v>
+      </c>
+      <c r="K24">
+        <v>129.30000000000001</v>
+      </c>
+      <c r="L24">
+        <f t="shared" ref="L24:L31" si="23">K24-C24</f>
+        <v>76.300000000000011</v>
+      </c>
+      <c r="M24">
+        <f t="shared" ref="M24:M31" si="24">ATAN(-300/B24)*3200/PI()</f>
+        <v>-76.25161473456032</v>
+      </c>
+      <c r="N24">
+        <v>-23.4</v>
+      </c>
+      <c r="O24">
+        <f t="shared" ref="O24:O31" si="25">N24-C24</f>
+        <v>-76.400000000000006</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>17</v>
       </c>
       <c r="B25">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6000</v>
+      </c>
+      <c r="C25">
+        <v>89.5</v>
+      </c>
+      <c r="D25">
+        <v>11</v>
+      </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+      <c r="F25">
+        <v>154</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="20"/>
+        <v>8.1119799797858601E-3</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="21"/>
+        <v>1.7136728465281196E-3</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="22"/>
+        <v>50.887204019764404</v>
+      </c>
+      <c r="K25">
+        <v>140.80000000000001</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="23"/>
+        <v>51.300000000000011</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="24"/>
+        <v>-50.887204019764404</v>
+      </c>
+      <c r="N25">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="25"/>
+        <v>-50.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
       <c r="B26">
         <f>ROUND(AVERAGE(B28,B24),-3)</f>
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8000</v>
+      </c>
+      <c r="C26">
+        <v>136.5</v>
+      </c>
+      <c r="D26">
+        <v>16</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <v>332</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="20"/>
+        <v>1.1019152667768446E-2</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="21"/>
+        <v>-5.4227025670370937E-4</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="22"/>
+        <v>38.179296503084508</v>
+      </c>
+      <c r="K26">
+        <v>175.1</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="23"/>
+        <v>38.599999999999994</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="24"/>
+        <v>-38.179296503084508</v>
+      </c>
+      <c r="N26">
+        <v>98.3</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="25"/>
+        <v>-38.200000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>17</v>
       </c>
       <c r="B27">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10000</v>
+      </c>
+      <c r="C27">
+        <v>197.3</v>
+      </c>
+      <c r="D27">
+        <v>22</v>
+      </c>
+      <c r="E27">
+        <v>8</v>
+      </c>
+      <c r="F27">
+        <v>637</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="20"/>
+        <v>1.1503422642719509E-2</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="21"/>
+        <v>-4.9564749233504532E-3</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="22"/>
+        <v>30.548586696097015</v>
+      </c>
+      <c r="K27">
+        <v>228.2</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="23"/>
+        <v>30.899999999999977</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="24"/>
+        <v>-30.548586696097015</v>
+      </c>
+      <c r="N27">
+        <v>166.6</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="25"/>
+        <v>-30.700000000000017</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>17</v>
       </c>
       <c r="B28">
-        <f>ROUND(AVERAGE(B32,B24),-3)</f>
-        <v>11000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>12000</v>
+      </c>
+      <c r="C28">
+        <v>274</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="20"/>
+        <v>-11.762196122315792</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="21"/>
+        <v>-2.5158097782635457E-2</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="22"/>
+        <v>25.459487718482603</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="23"/>
+        <v>-274</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="24"/>
+        <v>-25.459487718482603</v>
+      </c>
+      <c r="N28">
+        <v>247.9</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="25"/>
+        <v>-26.099999999999994</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>17</v>
       </c>
       <c r="B29">
-        <v>13000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>14000</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="20"/>
+        <v>-1</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="22"/>
+        <v>21.823623682391897</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="24"/>
+        <v>-21.823623682391897</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>17</v>
       </c>
       <c r="B30">
-        <f>ROUND(AVERAGE(B32,B28),-3)</f>
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>16000</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="20"/>
+        <v>-1</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="22"/>
+        <v>19.096355526624365</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="24"/>
+        <v>-19.096355526624365</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>17</v>
       </c>
       <c r="B31">
-        <v>16000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18000</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="20"/>
+        <v>-1</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="22"/>
+        <v>16.974955624394465</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="24"/>
+        <v>-16.974955624394465</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B32">
-        <v>18000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -3265,7 +4007,7 @@
         <v>18</v>
       </c>
       <c r="B33">
-        <v>3000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -3273,7 +4015,8 @@
         <v>18</v>
       </c>
       <c r="B34">
-        <v>6000</v>
+        <f>ROUND(AVERAGE(B36,B32),-3)</f>
+        <v>8000</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -3281,8 +4024,7 @@
         <v>18</v>
       </c>
       <c r="B35">
-        <f>ROUND(AVERAGE(B37,B33),-3)</f>
-        <v>8000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -3290,7 +4032,8 @@
         <v>18</v>
       </c>
       <c r="B36">
-        <v>10000</v>
+        <f>ROUND(AVERAGE(B40,B32),-3)</f>
+        <v>12000</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -3298,8 +4041,7 @@
         <v>18</v>
       </c>
       <c r="B37">
-        <f>ROUND(AVERAGE(B41,B33),-3)</f>
-        <v>12000</v>
+        <v>14000</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -3307,7 +4049,8 @@
         <v>18</v>
       </c>
       <c r="B38">
-        <v>14000</v>
+        <f>ROUND(AVERAGE(B40,B36),-3)</f>
+        <v>17000</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -3315,8 +4058,7 @@
         <v>18</v>
       </c>
       <c r="B39">
-        <f>ROUND(AVERAGE(B41,B37),-3)</f>
-        <v>17000</v>
+        <v>19000</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -3324,14 +4066,6 @@
         <v>18</v>
       </c>
       <c r="B40">
-        <v>19000</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>18</v>
-      </c>
-      <c r="B41">
         <v>21000</v>
       </c>
     </row>

</xml_diff>